<commit_message>
Update results.xlsx in beacon
</commit_message>
<xml_diff>
--- a/results/beacon/resultTable.xlsx
+++ b/results/beacon/resultTable.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="45">
   <si>
     <t>BookStackTest_1</t>
   </si>
@@ -118,13 +118,54 @@
   </si>
   <si>
     <t>ApproximateEntropy_7</t>
+  </si>
+  <si>
+    <t>BookStackTest_8_16</t>
+  </si>
+  <si>
+    <t>BookStackTest_16_16</t>
+  </si>
+  <si>
+    <t>BookStackTest_32_16</t>
+  </si>
+  <si>
+    <t>BookStackTest_16_256</t>
+  </si>
+  <si>
+    <t>BookStackTest_32_65536</t>
+  </si>
+  <si>
+    <t>BookStackTest_8_128</t>
+  </si>
+  <si>
+    <t>BookStackTest_16_32768</t>
+  </si>
+  <si>
+    <t>minstd_rand</t>
+  </si>
+  <si>
+    <t>256_Kbits</t>
+  </si>
+  <si>
+    <t>512_Kbits</t>
+  </si>
+  <si>
+    <t>ranlux48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,18 +192,291 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Результаты тестов на "истинной"</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>случайной последовательности</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Пройденные тесты</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$T$11:$AO$11</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>BookStackTest_1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BookStackTest_2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BookStackTest_3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BookStackTest_4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BookStackTest_5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BookStackTest_6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>BookStackTest_7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>BookStackTest_8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Frequency</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>BlockFrequency_5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Runs</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>LongestRunOfOnes</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Rank</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>DiscreteFourierTransform</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>NonOverlappingTemplateMatchings_5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>OverlappingTemplateMatchings_5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Universal</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>LinearComplexity_25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Serial_5_1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Serial_5_2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>ApproximateEntropy_7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>CumulativeSums_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$T$12:$AO$12</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="89091456"/>
+        <c:axId val="90771456"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="89091456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90771456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90771456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89091456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:AO60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -461,7 +775,7 @@
     <col min="4" max="4" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:41">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +852,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:41">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -618,7 +932,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:41">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -698,7 +1012,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:41">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -778,7 +1092,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:41">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -858,7 +1172,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:41">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -938,7 +1252,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:41">
       <c r="E10" t="s">
         <v>23</v>
       </c>
@@ -967,7 +1281,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:41">
+      <c r="C11" s="1">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
@@ -998,8 +1315,81 @@
       <c r="M11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="N11" s="1">
+        <f>AVERAGE(E11:M11)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="T11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>1</v>
+      </c>
+      <c r="V11" t="s">
+        <v>2</v>
+      </c>
+      <c r="W11" t="s">
+        <v>3</v>
+      </c>
+      <c r="X11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
       <c r="D12" t="s">
         <v>1</v>
       </c>
@@ -1030,8 +1420,81 @@
       <c r="M12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:26">
+      <c r="N12" s="1">
+        <f t="shared" ref="N12:N33" si="0">AVERAGE(E12:M12)</f>
+        <v>1</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="U12" s="1">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1">
+        <v>1</v>
+      </c>
+      <c r="W12" s="1">
+        <v>1</v>
+      </c>
+      <c r="X12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="AI12" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="1">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="AO12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41">
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
       <c r="D13" t="s">
         <v>2</v>
       </c>
@@ -1062,8 +1525,15 @@
       <c r="M13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:26">
+      <c r="N13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
       <c r="D14" t="s">
         <v>3</v>
       </c>
@@ -1094,8 +1564,15 @@
       <c r="M14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:26">
+      <c r="N14" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -1126,8 +1603,15 @@
       <c r="M15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:26">
+      <c r="N15" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41">
+      <c r="C16" s="1">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
@@ -1158,8 +1642,15 @@
       <c r="M16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="4:13">
+      <c r="N16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
@@ -1190,8 +1681,15 @@
       <c r="M17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="4:13">
+      <c r="N17" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14">
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
@@ -1222,8 +1720,15 @@
       <c r="M18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="4:13">
+      <c r="N18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
@@ -1254,8 +1759,15 @@
       <c r="M19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="4:13">
+      <c r="N19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
@@ -1286,8 +1798,15 @@
       <c r="M20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="4:13">
+      <c r="N20" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14">
+      <c r="C21" s="1">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
@@ -1318,8 +1837,15 @@
       <c r="M21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="4:13">
+      <c r="N21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
@@ -1350,8 +1876,15 @@
       <c r="M22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="4:13">
+      <c r="N22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14">
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
@@ -1382,8 +1915,15 @@
       <c r="M23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="4:13">
+      <c r="N23" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14">
+      <c r="C24" s="1">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
@@ -1414,8 +1954,15 @@
       <c r="M24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="4:13">
+      <c r="N24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14">
+      <c r="C25" s="1">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D25" t="s">
         <v>14</v>
       </c>
@@ -1446,8 +1993,15 @@
       <c r="M25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="4:13">
+      <c r="N25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14">
+      <c r="C26" s="1">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
@@ -1478,8 +2032,15 @@
       <c r="M26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="4:13">
+      <c r="N26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14">
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
       <c r="D27" t="s">
         <v>16</v>
       </c>
@@ -1510,8 +2071,15 @@
       <c r="M27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="4:13">
+      <c r="N27" s="1">
+        <f>AVERAGE(M27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14">
+      <c r="C28" s="1">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
@@ -1542,8 +2110,15 @@
       <c r="M28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="4:13">
+      <c r="N28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14">
+      <c r="C29" s="1">
+        <v>0.77777777777777779</v>
+      </c>
       <c r="D29" t="s">
         <v>18</v>
       </c>
@@ -1574,8 +2149,15 @@
       <c r="M29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="4:13">
+      <c r="N29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14">
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
       <c r="D30" t="s">
         <v>19</v>
       </c>
@@ -1606,8 +2188,15 @@
       <c r="M30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="4:13">
+      <c r="N30" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14">
+      <c r="C31" s="1">
+        <v>0.77777777777777779</v>
+      </c>
       <c r="D31" t="s">
         <v>33</v>
       </c>
@@ -1638,8 +2227,15 @@
       <c r="M31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="4:13">
+      <c r="N31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
       <c r="D32" t="s">
         <v>20</v>
       </c>
@@ -1670,8 +2266,12 @@
       <c r="M32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="4:13">
+      <c r="N32" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14">
       <c r="D33" t="s">
         <v>20</v>
       </c>
@@ -1702,8 +2302,9 @@
       <c r="M33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="4:13">
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="4:14">
       <c r="D34" t="s">
         <v>21</v>
       </c>
@@ -1735,7 +2336,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="4:13">
+    <row r="35" spans="4:14">
       <c r="D35" t="s">
         <v>22</v>
       </c>
@@ -1767,8 +2368,420 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="41" spans="4:14">
+      <c r="D41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="4:14">
+      <c r="E42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" t="s">
+        <v>38</v>
+      </c>
+      <c r="K42" t="s">
+        <v>39</v>
+      </c>
+      <c r="L42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="4:14">
+      <c r="D43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:14">
+      <c r="D44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:14">
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>6</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="4:14">
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:12">
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="4:12">
+      <c r="E52" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" t="s">
+        <v>36</v>
+      </c>
+      <c r="H52" t="s">
+        <v>34</v>
+      </c>
+      <c r="I52" t="s">
+        <v>37</v>
+      </c>
+      <c r="J52" t="s">
+        <v>38</v>
+      </c>
+      <c r="K52" t="s">
+        <v>39</v>
+      </c>
+      <c r="L52" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="4:12">
+      <c r="D53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:12">
+      <c r="D54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:12">
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:12">
+      <c r="D56" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>2</v>
+      </c>
+      <c r="L56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="4:12">
+      <c r="D57" t="s">
+        <v>31</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>9</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:12">
+      <c r="D58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>5</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>10</v>
+      </c>
+      <c r="J58">
+        <v>2</v>
+      </c>
+      <c r="K58">
+        <v>2</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:12">
+      <c r="D59" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>6</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>10</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="4:12">
+      <c r="D60" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>9</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>10</v>
+      </c>
+      <c r="J60">
+        <v>4</v>
+      </c>
+      <c r="K60">
+        <v>3</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>